<commit_message>
Implementado algorimto que elimina las nuevas ITVs no rentables.
</commit_message>
<xml_diff>
--- a/CLM_Datos.xlsx
+++ b/CLM_Datos.xlsx
@@ -2900,8 +2900,8 @@
   </sheetPr>
   <dimension ref="A1:K919"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L9" activeCellId="0" sqref="L9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A874" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K121" activeCellId="0" sqref="K121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14002,7 +14002,9 @@
       <c r="I346" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="J346" s="1"/>
+      <c r="J346" s="1" t="n">
+        <v>247</v>
+      </c>
     </row>
     <row r="347" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="0" t="s">

</xml_diff>